<commit_message>
Added booking CRUD tests with token and authorization handling for Restful-Booker API
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceqin/IntelliJ projects/Api-Testing-Framework-Restassured/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4408D87B-0AFF-9841-89C7-6DF7EBD22AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A39E95-4F95-6646-9F04-73CD85373001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="8720" windowWidth="27460" windowHeight="16940" activeTab="1" xr2:uid="{23DFC228-E359-8440-9892-7C89A6F9F649}"/>
+    <workbookView xWindow="1340" yWindow="1060" windowWidth="27460" windowHeight="16940" activeTab="1" xr2:uid="{23DFC228-E359-8440-9892-7C89A6F9F649}"/>
   </bookViews>
   <sheets>
     <sheet name="Signup" sheetId="1" r:id="rId1"/>
@@ -548,13 +548,14 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="4" width="21" customWidth="1"/>
+    <col min="3" max="3" width="21" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>